<commit_message>
Atualização de nomes de algumas variáveis
</commit_message>
<xml_diff>
--- a/sf_weather.xlsx
+++ b/sf_weather.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
   <si>
     <t>period</t>
   </si>
@@ -61,27 +61,21 @@
     <t>Tuesday</t>
   </si>
   <si>
-    <t>Mostly Sunnythen Sunnyand Breezy</t>
-  </si>
-  <si>
-    <t>Partly Cloudy</t>
-  </si>
-  <si>
     <t>BecomingSunny</t>
   </si>
   <si>
+    <t>Mostly Clear</t>
+  </si>
+  <si>
     <t>Mostly Clearand Breezythen PartlyCloudy</t>
   </si>
   <si>
+    <t>Mostly Sunny</t>
+  </si>
+  <si>
     <t>Sunny</t>
   </si>
   <si>
-    <t>Mostly Clear</t>
-  </si>
-  <si>
-    <t>Mostly Sunny</t>
-  </si>
-  <si>
     <t>High: 73 °F</t>
   </si>
   <si>
@@ -100,10 +94,10 @@
     <t>High: 71 °F</t>
   </si>
   <si>
-    <t xml:space="preserve">Today: Partly sunny, then gradually becoming sunny, with a high near 73. Breezy, with a west southwest wind 6 to 11 mph increasing to 17 to 22 mph in the afternoon. Winds could gust as high as 29 mph. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tonight: Partly cloudy, with a low around 59. West southwest wind 9 to 18 mph, with gusts as high as 23 mph. </t>
+    <t xml:space="preserve">Today: Partly sunny, then gradually becoming sunny, with a high near 73. West southwest wind 6 to 11 mph increasing to 16 to 21 mph in the afternoon. Winds could gust as high as 26 mph. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tonight: Mostly clear, with a low around 59. Southwest wind 16 to 21 mph decreasing to 9 to 14 mph after midnight. Winds could gust as high as 28 mph. </t>
   </si>
   <si>
     <t xml:space="preserve">Saturday: Partly sunny, then gradually becoming sunny, with a high near 75. West southwest wind 5 to 10 mph increasing to 16 to 21 mph in the afternoon. Winds could gust as high as 26 mph. </t>
@@ -112,7 +106,7 @@
     <t xml:space="preserve">Saturday Night: Mostly clear, with a low around 58. Breezy, with a west southwest wind 15 to 22 mph, with gusts as high as 29 mph. </t>
   </si>
   <si>
-    <t xml:space="preserve">Sunday: Sunny, with a high near 70. Southwest wind 17 to 21 mph, with gusts as high as 28 mph. </t>
+    <t xml:space="preserve">Sunday: Mostly sunny, with a high near 70. Southwest wind 17 to 21 mph, with gusts as high as 28 mph. </t>
   </si>
   <si>
     <t>Sunday Night: Mostly clear, with a low around 59.</t>
@@ -121,7 +115,7 @@
     <t>Monday: Sunny, with a high near 75.</t>
   </si>
   <si>
-    <t>Monday Night: Partly cloudy, with a low around 59.</t>
+    <t>Monday Night: Mostly clear, with a low around 59.</t>
   </si>
   <si>
     <t>Tuesday: Mostly sunny, with a high near 71.</t>
@@ -519,10 +513,10 @@
         <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F2">
         <v>73</v>
@@ -542,10 +536,10 @@
         <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F3">
         <v>59</v>
@@ -562,13 +556,13 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F4">
         <v>75</v>
@@ -585,13 +579,13 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F5">
         <v>58</v>
@@ -608,13 +602,13 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F6">
         <v>70</v>
@@ -631,13 +625,13 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F7">
         <v>59</v>
@@ -657,10 +651,10 @@
         <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F8">
         <v>75</v>
@@ -680,10 +674,10 @@
         <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F9">
         <v>59</v>
@@ -700,13 +694,13 @@
         <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F10">
         <v>71</v>

</xml_diff>